<commit_message>
jeddah and vegas points
</commit_message>
<xml_diff>
--- a/The_Alternative_F1.xlsx
+++ b/The_Alternative_F1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1837" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="309">
   <si>
     <t>Positions</t>
   </si>
@@ -922,25 +922,19 @@
     <t>12/17/2025</t>
   </si>
   <si>
-    <t>Confirmed</t>
-  </si>
-  <si>
     <t>Jeddah</t>
   </si>
   <si>
-    <t>1/1/2026</t>
+    <t>1/7/2026</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>1/14/2026</t>
   </si>
   <si>
     <t>Tentative</t>
-  </si>
-  <si>
-    <t>Las Vegas</t>
-  </si>
-  <si>
-    <t>1/7/2026</t>
-  </si>
-  <si>
-    <t>1/14/2026</t>
   </si>
   <si>
     <t>Imola</t>
@@ -2085,29 +2079,29 @@
         <v>299</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B16" s="93" t="s">
         <v>301</v>
       </c>
-      <c r="B16" s="93" t="s">
-        <v>302</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B17" s="93" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
     </row>
     <row r="18">
@@ -2115,32 +2109,32 @@
         <v>159</v>
       </c>
       <c r="B18" s="93" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B19" s="93" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B20" s="93" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -10491,25 +10485,49 @@
         <f>IFERROR((VLOOKUP(CJ2,Scoring!$A:$B,2,0))+IF(CL2="y",1,0)+IF(CM2="y",1,0)+IF(CN2="y",1,0)+IF(CO2="y",1,0),0)</f>
         <v>26</v>
       </c>
-      <c r="CQ2" s="15"/>
-      <c r="CR2" s="23"/>
-      <c r="CS2" s="24"/>
-      <c r="CT2" s="25"/>
-      <c r="CU2" s="26"/>
-      <c r="CV2" s="27"/>
+      <c r="CQ2" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="CR2" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="CS2" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="CT2" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="CU2" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="CV2" s="11" t="s">
+        <v>279</v>
+      </c>
       <c r="CW2" s="21">
         <f>IFERROR((VLOOKUP(CQ2,Scoring!$A:$B,2,0))+IF(CS2="y",1,0)+IF(CT2="y",1,0)+IF(CU2="y",1,0)+IF(CV2="y",1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CX2" s="15"/>
-      <c r="CY2" s="23"/>
-      <c r="CZ2" s="24"/>
-      <c r="DA2" s="25"/>
-      <c r="DB2" s="26"/>
-      <c r="DC2" s="27"/>
+        <v>26</v>
+      </c>
+      <c r="CX2" s="15">
+        <v>5.0</v>
+      </c>
+      <c r="CY2" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="CZ2" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="DA2" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="DB2" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="DC2" s="11" t="s">
+        <v>279</v>
+      </c>
       <c r="DD2" s="21">
         <f>IFERROR((VLOOKUP(CX2,Scoring!$A:$B,2,0))+IF(CZ2="y",1,0)+IF(DA2="y",1,0)+IF(DB2="y",1,0)+IF(DC2="y",1,0),0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="DE2" s="15"/>
       <c r="DF2" s="23"/>
@@ -10828,22 +10846,46 @@
         <f>IFERROR((VLOOKUP(CJ3,Scoring!$A:$B,2,0))+IF(CL3="y",1,0)+IF(CM3="y",1,0)+IF(CN3="y",1,0)+IF(CO3="y",1,0),0)</f>
         <v>1</v>
       </c>
-      <c r="CQ3" s="28"/>
-      <c r="CR3" s="37"/>
-      <c r="CS3" s="38"/>
-      <c r="CT3" s="39"/>
-      <c r="CU3" s="40"/>
-      <c r="CV3" s="41"/>
+      <c r="CQ3" s="28">
+        <v>7.0</v>
+      </c>
+      <c r="CR3" s="29">
+        <v>14.0</v>
+      </c>
+      <c r="CS3" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="CT3" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="CU3" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="CV3" s="36" t="s">
+        <v>279</v>
+      </c>
       <c r="CW3" s="34">
         <f>IFERROR((VLOOKUP(CQ3,Scoring!$A:$B,2,0))+IF(CS3="y",1,0)+IF(CT3="y",1,0)+IF(CU3="y",1,0)+IF(CV3="y",1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CX3" s="28"/>
-      <c r="CY3" s="37"/>
-      <c r="CZ3" s="38"/>
-      <c r="DA3" s="39"/>
-      <c r="DB3" s="40"/>
-      <c r="DC3" s="41"/>
+        <v>6</v>
+      </c>
+      <c r="CX3" s="28">
+        <v>22.0</v>
+      </c>
+      <c r="CY3" s="29">
+        <v>22.0</v>
+      </c>
+      <c r="CZ3" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="DA3" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="DB3" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="DC3" s="36" t="s">
+        <v>279</v>
+      </c>
       <c r="DD3" s="34">
         <f>IFERROR((VLOOKUP(CX3,Scoring!$A:$B,2,0))+IF(CZ3="y",1,0)+IF(DA3="y",1,0)+IF(DB3="y",1,0)+IF(DC3="y",1,0),0)</f>
         <v>0</v>
@@ -11165,25 +11207,49 @@
         <f>IFERROR((VLOOKUP(CJ4,Scoring!$A:$B,2,0))+IF(CL4="y",1,0)+IF(CM4="y",1,0)+IF(CN4="y",1,0)+IF(CO4="y",1,0),0)</f>
         <v>12</v>
       </c>
-      <c r="CQ4" s="45"/>
-      <c r="CR4" s="54"/>
-      <c r="CS4" s="55"/>
-      <c r="CT4" s="56"/>
-      <c r="CU4" s="57"/>
-      <c r="CV4" s="58"/>
+      <c r="CQ4" s="45">
+        <v>4.0</v>
+      </c>
+      <c r="CR4" s="46">
+        <v>15.0</v>
+      </c>
+      <c r="CS4" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="CT4" s="48" t="s">
+        <v>278</v>
+      </c>
+      <c r="CU4" s="49" t="s">
+        <v>278</v>
+      </c>
+      <c r="CV4" s="53" t="s">
+        <v>279</v>
+      </c>
       <c r="CW4" s="51">
         <f>IFERROR((VLOOKUP(CQ4,Scoring!$A:$B,2,0))+IF(CS4="y",1,0)+IF(CT4="y",1,0)+IF(CU4="y",1,0)+IF(CV4="y",1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CX4" s="45"/>
-      <c r="CY4" s="54"/>
-      <c r="CZ4" s="55"/>
-      <c r="DA4" s="56"/>
-      <c r="DB4" s="57"/>
-      <c r="DC4" s="58"/>
+        <v>14</v>
+      </c>
+      <c r="CX4" s="45">
+        <v>3.0</v>
+      </c>
+      <c r="CY4" s="46">
+        <v>3.0</v>
+      </c>
+      <c r="CZ4" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="DA4" s="48" t="s">
+        <v>279</v>
+      </c>
+      <c r="DB4" s="49" t="s">
+        <v>279</v>
+      </c>
+      <c r="DC4" s="53" t="s">
+        <v>279</v>
+      </c>
       <c r="DD4" s="51">
         <f>IFERROR((VLOOKUP(CX4,Scoring!$A:$B,2,0))+IF(CZ4="y",1,0)+IF(DA4="y",1,0)+IF(DB4="y",1,0)+IF(DC4="y",1,0),0)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="DE4" s="45"/>
       <c r="DF4" s="54"/>
@@ -11502,22 +11568,46 @@
         <f>IFERROR((VLOOKUP(CJ5,Scoring!$A:$B,2,0))+IF(CL5="y",1,0)+IF(CM5="y",1,0)+IF(CN5="y",1,0)+IF(CO5="y",1,0),0)</f>
         <v>0</v>
       </c>
-      <c r="CQ5" s="62"/>
-      <c r="CR5" s="71"/>
-      <c r="CS5" s="72"/>
-      <c r="CT5" s="73"/>
-      <c r="CU5" s="74"/>
-      <c r="CV5" s="75"/>
+      <c r="CQ5" s="62">
+        <v>22.0</v>
+      </c>
+      <c r="CR5" s="63">
+        <v>22.0</v>
+      </c>
+      <c r="CS5" s="64" t="s">
+        <v>279</v>
+      </c>
+      <c r="CT5" s="65" t="s">
+        <v>279</v>
+      </c>
+      <c r="CU5" s="66" t="s">
+        <v>279</v>
+      </c>
+      <c r="CV5" s="70" t="s">
+        <v>279</v>
+      </c>
       <c r="CW5" s="68">
         <f>IFERROR((VLOOKUP(CQ5,Scoring!$A:$B,2,0))+IF(CS5="y",1,0)+IF(CT5="y",1,0)+IF(CU5="y",1,0)+IF(CV5="y",1,0),0)</f>
         <v>0</v>
       </c>
-      <c r="CX5" s="62"/>
-      <c r="CY5" s="71"/>
-      <c r="CZ5" s="72"/>
-      <c r="DA5" s="73"/>
-      <c r="DB5" s="74"/>
-      <c r="DC5" s="75"/>
+      <c r="CX5" s="62">
+        <v>22.0</v>
+      </c>
+      <c r="CY5" s="63">
+        <v>22.0</v>
+      </c>
+      <c r="CZ5" s="64" t="s">
+        <v>279</v>
+      </c>
+      <c r="DA5" s="65" t="s">
+        <v>279</v>
+      </c>
+      <c r="DB5" s="66" t="s">
+        <v>279</v>
+      </c>
+      <c r="DC5" s="70" t="s">
+        <v>279</v>
+      </c>
       <c r="DD5" s="68">
         <f>IFERROR((VLOOKUP(CX5,Scoring!$A:$B,2,0))+IF(CZ5="y",1,0)+IF(DA5="y",1,0)+IF(DB5="y",1,0)+IF(DC5="y",1,0),0)</f>
         <v>0</v>
@@ -11839,25 +11929,49 @@
         <f>IFERROR((VLOOKUP(CJ6,Scoring!$A:$B,2,0))+IF(CL6="y",1,0)+IF(CM6="y",1,0)+IF(CN6="y",1,0)+IF(CO6="y",1,0),0)</f>
         <v>18</v>
       </c>
-      <c r="CQ6" s="28"/>
-      <c r="CR6" s="37"/>
-      <c r="CS6" s="38"/>
-      <c r="CT6" s="39"/>
-      <c r="CU6" s="40"/>
-      <c r="CV6" s="41"/>
+      <c r="CQ6" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="CR6" s="29">
+        <v>5.0</v>
+      </c>
+      <c r="CS6" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="CT6" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="CU6" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="CV6" s="36" t="s">
+        <v>278</v>
+      </c>
       <c r="CW6" s="34">
         <f>IFERROR((VLOOKUP(CQ6,Scoring!$A:$B,2,0))+IF(CS6="y",1,0)+IF(CT6="y",1,0)+IF(CU6="y",1,0)+IF(CV6="y",1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CX6" s="28"/>
-      <c r="CY6" s="37"/>
-      <c r="CZ6" s="38"/>
-      <c r="DA6" s="39"/>
-      <c r="DB6" s="40"/>
-      <c r="DC6" s="41"/>
+        <v>19</v>
+      </c>
+      <c r="CX6" s="28">
+        <v>2.0</v>
+      </c>
+      <c r="CY6" s="29">
+        <v>4.0</v>
+      </c>
+      <c r="CZ6" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="DA6" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="DB6" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="DC6" s="36" t="s">
+        <v>278</v>
+      </c>
       <c r="DD6" s="34">
         <f>IFERROR((VLOOKUP(CX6,Scoring!$A:$B,2,0))+IF(CZ6="y",1,0)+IF(DA6="y",1,0)+IF(DB6="y",1,0)+IF(DC6="y",1,0),0)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="DE6" s="28"/>
       <c r="DF6" s="37"/>
@@ -12176,22 +12290,46 @@
         <f>IFERROR((VLOOKUP(CJ7,Scoring!$A:$B,2,0))+IF(CL7="y",1,0)+IF(CM7="y",1,0)+IF(CN7="y",1,0)+IF(CO7="y",1,0),0)</f>
         <v>10</v>
       </c>
-      <c r="CQ7" s="28"/>
-      <c r="CR7" s="37"/>
-      <c r="CS7" s="38"/>
-      <c r="CT7" s="39"/>
-      <c r="CU7" s="40"/>
-      <c r="CV7" s="41"/>
+      <c r="CQ7" s="28">
+        <v>3.0</v>
+      </c>
+      <c r="CR7" s="29">
+        <v>6.0</v>
+      </c>
+      <c r="CS7" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="CT7" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="CU7" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="CV7" s="36" t="s">
+        <v>279</v>
+      </c>
       <c r="CW7" s="34">
         <f>IFERROR((VLOOKUP(CQ7,Scoring!$A:$B,2,0))+IF(CS7="y",1,0)+IF(CT7="y",1,0)+IF(CU7="y",1,0)+IF(CV7="y",1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CX7" s="28"/>
-      <c r="CY7" s="37"/>
-      <c r="CZ7" s="38"/>
-      <c r="DA7" s="39"/>
-      <c r="DB7" s="40"/>
-      <c r="DC7" s="41"/>
+        <v>15</v>
+      </c>
+      <c r="CX7" s="28">
+        <v>21.0</v>
+      </c>
+      <c r="CY7" s="29">
+        <v>5.0</v>
+      </c>
+      <c r="CZ7" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="DA7" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="DB7" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="DC7" s="36" t="s">
+        <v>279</v>
+      </c>
       <c r="DD7" s="34">
         <f>IFERROR((VLOOKUP(CX7,Scoring!$A:$B,2,0))+IF(CZ7="y",1,0)+IF(DA7="y",1,0)+IF(DB7="y",1,0)+IF(DC7="y",1,0),0)</f>
         <v>0</v>
@@ -12513,22 +12651,46 @@
         <f>IFERROR((VLOOKUP(CJ8,Scoring!$A:$B,2,0))+IF(CL8="y",1,0)+IF(CM8="y",1,0)+IF(CN8="y",1,0)+IF(CO8="y",1,0),0)</f>
         <v>3</v>
       </c>
-      <c r="CQ8" s="45"/>
-      <c r="CR8" s="54"/>
-      <c r="CS8" s="55"/>
-      <c r="CT8" s="56"/>
-      <c r="CU8" s="57"/>
-      <c r="CV8" s="58"/>
+      <c r="CQ8" s="45">
+        <v>22.0</v>
+      </c>
+      <c r="CR8" s="46">
+        <v>22.0</v>
+      </c>
+      <c r="CS8" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="CT8" s="48" t="s">
+        <v>279</v>
+      </c>
+      <c r="CU8" s="49" t="s">
+        <v>279</v>
+      </c>
+      <c r="CV8" s="53" t="s">
+        <v>279</v>
+      </c>
       <c r="CW8" s="51">
         <f>IFERROR((VLOOKUP(CQ8,Scoring!$A:$B,2,0))+IF(CS8="y",1,0)+IF(CT8="y",1,0)+IF(CU8="y",1,0)+IF(CV8="y",1,0),0)</f>
         <v>0</v>
       </c>
-      <c r="CX8" s="45"/>
-      <c r="CY8" s="54"/>
-      <c r="CZ8" s="55"/>
-      <c r="DA8" s="56"/>
-      <c r="DB8" s="57"/>
-      <c r="DC8" s="58"/>
+      <c r="CX8" s="45">
+        <v>22.0</v>
+      </c>
+      <c r="CY8" s="46">
+        <v>22.0</v>
+      </c>
+      <c r="CZ8" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="DA8" s="48" t="s">
+        <v>279</v>
+      </c>
+      <c r="DB8" s="49" t="s">
+        <v>279</v>
+      </c>
+      <c r="DC8" s="53" t="s">
+        <v>279</v>
+      </c>
       <c r="DD8" s="51">
         <f>IFERROR((VLOOKUP(CX8,Scoring!$A:$B,2,0))+IF(CZ8="y",1,0)+IF(DA8="y",1,0)+IF(DB8="y",1,0)+IF(DC8="y",1,0),0)</f>
         <v>0</v>
@@ -12850,22 +13012,46 @@
         <f>IFERROR((VLOOKUP(CJ9,Scoring!$A:$B,2,0))+IF(CL9="y",1,0)+IF(CM9="y",1,0)+IF(CN9="y",1,0)+IF(CO9="y",1,0),0)</f>
         <v>8</v>
       </c>
-      <c r="CQ9" s="62"/>
-      <c r="CR9" s="71"/>
-      <c r="CS9" s="72"/>
-      <c r="CT9" s="73"/>
-      <c r="CU9" s="74"/>
-      <c r="CV9" s="75"/>
+      <c r="CQ9" s="62">
+        <v>11.0</v>
+      </c>
+      <c r="CR9" s="63">
+        <v>4.0</v>
+      </c>
+      <c r="CS9" s="64" t="s">
+        <v>279</v>
+      </c>
+      <c r="CT9" s="65" t="s">
+        <v>279</v>
+      </c>
+      <c r="CU9" s="66" t="s">
+        <v>279</v>
+      </c>
+      <c r="CV9" s="70" t="s">
+        <v>279</v>
+      </c>
       <c r="CW9" s="68">
         <f>IFERROR((VLOOKUP(CQ9,Scoring!$A:$B,2,0))+IF(CS9="y",1,0)+IF(CT9="y",1,0)+IF(CU9="y",1,0)+IF(CV9="y",1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CX9" s="62"/>
-      <c r="CY9" s="71"/>
-      <c r="CZ9" s="72"/>
-      <c r="DA9" s="73"/>
-      <c r="DB9" s="74"/>
-      <c r="DC9" s="75"/>
+        <v>1</v>
+      </c>
+      <c r="CX9" s="62">
+        <v>21.0</v>
+      </c>
+      <c r="CY9" s="63">
+        <v>8.0</v>
+      </c>
+      <c r="CZ9" s="64" t="s">
+        <v>279</v>
+      </c>
+      <c r="DA9" s="65" t="s">
+        <v>279</v>
+      </c>
+      <c r="DB9" s="66" t="s">
+        <v>279</v>
+      </c>
+      <c r="DC9" s="70" t="s">
+        <v>279</v>
+      </c>
       <c r="DD9" s="68">
         <f>IFERROR((VLOOKUP(CX9,Scoring!$A:$B,2,0))+IF(CZ9="y",1,0)+IF(DA9="y",1,0)+IF(DB9="y",1,0)+IF(DC9="y",1,0),0)</f>
         <v>0</v>
@@ -13187,25 +13373,49 @@
         <f>IFERROR((VLOOKUP(CJ10,Scoring!$A:$B,2,0))+IF(CL10="y",1,0)+IF(CM10="y",1,0)+IF(CN10="y",1,0)+IF(CO10="y",1,0),0)</f>
         <v>6</v>
       </c>
-      <c r="CQ10" s="28"/>
-      <c r="CR10" s="37"/>
-      <c r="CS10" s="38"/>
-      <c r="CT10" s="39"/>
-      <c r="CU10" s="40"/>
-      <c r="CV10" s="41"/>
+      <c r="CQ10" s="28">
+        <v>21.0</v>
+      </c>
+      <c r="CR10" s="29">
+        <v>3.0</v>
+      </c>
+      <c r="CS10" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="CT10" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="CU10" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="CV10" s="36" t="s">
+        <v>279</v>
+      </c>
       <c r="CW10" s="34">
         <f>IFERROR((VLOOKUP(CQ10,Scoring!$A:$B,2,0))+IF(CS10="y",1,0)+IF(CT10="y",1,0)+IF(CU10="y",1,0)+IF(CV10="y",1,0),0)</f>
         <v>0</v>
       </c>
-      <c r="CX10" s="28"/>
-      <c r="CY10" s="37"/>
-      <c r="CZ10" s="38"/>
-      <c r="DA10" s="39"/>
-      <c r="DB10" s="40"/>
-      <c r="DC10" s="41"/>
+      <c r="CX10" s="28">
+        <v>7.0</v>
+      </c>
+      <c r="CY10" s="29">
+        <v>7.0</v>
+      </c>
+      <c r="CZ10" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="DA10" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="DB10" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="DC10" s="36" t="s">
+        <v>279</v>
+      </c>
       <c r="DD10" s="34">
         <f>IFERROR((VLOOKUP(CX10,Scoring!$A:$B,2,0))+IF(CZ10="y",1,0)+IF(DA10="y",1,0)+IF(DB10="y",1,0)+IF(DC10="y",1,0),0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="DE10" s="28"/>
       <c r="DF10" s="37"/>
@@ -13524,22 +13734,46 @@
         <f>IFERROR((VLOOKUP(CJ11,Scoring!$A:$B,2,0))+IF(CL11="y",1,0)+IF(CM11="y",1,0)+IF(CN11="y",1,0)+IF(CO11="y",1,0),0)</f>
         <v>1</v>
       </c>
-      <c r="CQ11" s="28"/>
-      <c r="CR11" s="37"/>
-      <c r="CS11" s="38"/>
-      <c r="CT11" s="39"/>
-      <c r="CU11" s="40"/>
-      <c r="CV11" s="41"/>
+      <c r="CQ11" s="28">
+        <v>22.0</v>
+      </c>
+      <c r="CR11" s="29">
+        <v>22.0</v>
+      </c>
+      <c r="CS11" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="CT11" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="CU11" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="CV11" s="36" t="s">
+        <v>279</v>
+      </c>
       <c r="CW11" s="34">
         <f>IFERROR((VLOOKUP(CQ11,Scoring!$A:$B,2,0))+IF(CS11="y",1,0)+IF(CT11="y",1,0)+IF(CU11="y",1,0)+IF(CV11="y",1,0),0)</f>
         <v>0</v>
       </c>
-      <c r="CX11" s="28"/>
-      <c r="CY11" s="37"/>
-      <c r="CZ11" s="38"/>
-      <c r="DA11" s="39"/>
-      <c r="DB11" s="40"/>
-      <c r="DC11" s="41"/>
+      <c r="CX11" s="28">
+        <v>22.0</v>
+      </c>
+      <c r="CY11" s="29">
+        <v>22.0</v>
+      </c>
+      <c r="CZ11" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="DA11" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="DB11" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="DC11" s="36" t="s">
+        <v>279</v>
+      </c>
       <c r="DD11" s="34">
         <f>IFERROR((VLOOKUP(CX11,Scoring!$A:$B,2,0))+IF(CZ11="y",1,0)+IF(DA11="y",1,0)+IF(DB11="y",1,0)+IF(DC11="y",1,0),0)</f>
         <v>0</v>
@@ -13861,25 +14095,49 @@
         <f>IFERROR((VLOOKUP(CJ12,Scoring!$A:$B,2,0))+IF(CL12="y",1,0)+IF(CM12="y",1,0)+IF(CN12="y",1,0)+IF(CO12="y",1,0),0)</f>
         <v>3</v>
       </c>
-      <c r="CQ12" s="45"/>
-      <c r="CR12" s="54"/>
-      <c r="CS12" s="55"/>
-      <c r="CT12" s="56"/>
-      <c r="CU12" s="57"/>
-      <c r="CV12" s="58"/>
+      <c r="CQ12" s="45">
+        <v>5.0</v>
+      </c>
+      <c r="CR12" s="46">
+        <v>7.0</v>
+      </c>
+      <c r="CS12" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="CT12" s="48" t="s">
+        <v>279</v>
+      </c>
+      <c r="CU12" s="49" t="s">
+        <v>279</v>
+      </c>
+      <c r="CV12" s="53" t="s">
+        <v>279</v>
+      </c>
       <c r="CW12" s="51">
         <f>IFERROR((VLOOKUP(CQ12,Scoring!$A:$B,2,0))+IF(CS12="y",1,0)+IF(CT12="y",1,0)+IF(CU12="y",1,0)+IF(CV12="y",1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CX12" s="45"/>
-      <c r="CY12" s="54"/>
-      <c r="CZ12" s="55"/>
-      <c r="DA12" s="56"/>
-      <c r="DB12" s="57"/>
-      <c r="DC12" s="58"/>
+        <v>10</v>
+      </c>
+      <c r="CX12" s="45">
+        <v>6.0</v>
+      </c>
+      <c r="CY12" s="46">
+        <v>6.0</v>
+      </c>
+      <c r="CZ12" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="DA12" s="48" t="s">
+        <v>279</v>
+      </c>
+      <c r="DB12" s="49" t="s">
+        <v>279</v>
+      </c>
+      <c r="DC12" s="53" t="s">
+        <v>279</v>
+      </c>
       <c r="DD12" s="51">
         <f>IFERROR((VLOOKUP(CX12,Scoring!$A:$B,2,0))+IF(CZ12="y",1,0)+IF(DA12="y",1,0)+IF(DB12="y",1,0)+IF(DC12="y",1,0),0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="DE12" s="45"/>
       <c r="DF12" s="54"/>
@@ -14198,25 +14456,49 @@
         <f>IFERROR((VLOOKUP(CJ13,Scoring!$A:$B,2,0))+IF(CL13="y",1,0)+IF(CM13="y",1,0)+IF(CN13="y",1,0)+IF(CO13="y",1,0),0)</f>
         <v>4</v>
       </c>
-      <c r="CQ13" s="62"/>
-      <c r="CR13" s="71"/>
-      <c r="CS13" s="72"/>
-      <c r="CT13" s="73"/>
-      <c r="CU13" s="74"/>
-      <c r="CV13" s="75"/>
+      <c r="CQ13" s="62">
+        <v>6.0</v>
+      </c>
+      <c r="CR13" s="63">
+        <v>22.0</v>
+      </c>
+      <c r="CS13" s="64" t="s">
+        <v>279</v>
+      </c>
+      <c r="CT13" s="65" t="s">
+        <v>279</v>
+      </c>
+      <c r="CU13" s="66" t="s">
+        <v>279</v>
+      </c>
+      <c r="CV13" s="70" t="s">
+        <v>279</v>
+      </c>
       <c r="CW13" s="68">
         <f>IFERROR((VLOOKUP(CQ13,Scoring!$A:$B,2,0))+IF(CS13="y",1,0)+IF(CT13="y",1,0)+IF(CU13="y",1,0)+IF(CV13="y",1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CX13" s="62"/>
-      <c r="CY13" s="71"/>
-      <c r="CZ13" s="72"/>
-      <c r="DA13" s="73"/>
-      <c r="DB13" s="74"/>
-      <c r="DC13" s="75"/>
+        <v>8</v>
+      </c>
+      <c r="CX13" s="62">
+        <v>4.0</v>
+      </c>
+      <c r="CY13" s="63">
+        <v>9.0</v>
+      </c>
+      <c r="CZ13" s="64" t="s">
+        <v>279</v>
+      </c>
+      <c r="DA13" s="65" t="s">
+        <v>279</v>
+      </c>
+      <c r="DB13" s="66" t="s">
+        <v>278</v>
+      </c>
+      <c r="DC13" s="70" t="s">
+        <v>279</v>
+      </c>
       <c r="DD13" s="68">
         <f>IFERROR((VLOOKUP(CX13,Scoring!$A:$B,2,0))+IF(CZ13="y",1,0)+IF(DA13="y",1,0)+IF(DB13="y",1,0)+IF(DC13="y",1,0),0)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="DE13" s="62"/>
       <c r="DF13" s="71"/>
@@ -14535,22 +14817,46 @@
         <f>IFERROR((VLOOKUP(CJ14,Scoring!$A:$B,2,0))+IF(CL14="y",1,0)+IF(CM14="y",1,0)+IF(CN14="y",1,0)+IF(CO14="y",1,0),0)</f>
         <v>16</v>
       </c>
-      <c r="CQ14" s="28"/>
-      <c r="CR14" s="37"/>
-      <c r="CS14" s="38"/>
-      <c r="CT14" s="39"/>
-      <c r="CU14" s="40"/>
-      <c r="CV14" s="41"/>
+      <c r="CQ14" s="28">
+        <v>22.0</v>
+      </c>
+      <c r="CR14" s="29">
+        <v>22.0</v>
+      </c>
+      <c r="CS14" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="CT14" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="CU14" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="CV14" s="36" t="s">
+        <v>279</v>
+      </c>
       <c r="CW14" s="34">
         <f>IFERROR((VLOOKUP(CQ14,Scoring!$A:$B,2,0))+IF(CS14="y",1,0)+IF(CT14="y",1,0)+IF(CU14="y",1,0)+IF(CV14="y",1,0),0)</f>
         <v>0</v>
       </c>
-      <c r="CX14" s="28"/>
-      <c r="CY14" s="37"/>
-      <c r="CZ14" s="38"/>
-      <c r="DA14" s="39"/>
-      <c r="DB14" s="40"/>
-      <c r="DC14" s="41"/>
+      <c r="CX14" s="28">
+        <v>22.0</v>
+      </c>
+      <c r="CY14" s="29">
+        <v>22.0</v>
+      </c>
+      <c r="CZ14" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="DA14" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="DB14" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="DC14" s="36" t="s">
+        <v>279</v>
+      </c>
       <c r="DD14" s="34">
         <f>IFERROR((VLOOKUP(CX14,Scoring!$A:$B,2,0))+IF(CZ14="y",1,0)+IF(DA14="y",1,0)+IF(DB14="y",1,0)+IF(DC14="y",1,0),0)</f>
         <v>0</v>
@@ -14872,25 +15178,49 @@
         <f>IFERROR((VLOOKUP(CJ15,Scoring!$A:$B,2,0))+IF(CL15="y",1,0)+IF(CM15="y",1,0)+IF(CN15="y",1,0)+IF(CO15="y",1,0),0)</f>
         <v>2</v>
       </c>
-      <c r="CQ15" s="79"/>
-      <c r="CR15" s="88"/>
-      <c r="CS15" s="89"/>
-      <c r="CT15" s="90"/>
-      <c r="CU15" s="91"/>
-      <c r="CV15" s="92"/>
+      <c r="CQ15" s="79">
+        <v>9.0</v>
+      </c>
+      <c r="CR15" s="80">
+        <v>1.0</v>
+      </c>
+      <c r="CS15" s="81" t="s">
+        <v>279</v>
+      </c>
+      <c r="CT15" s="82" t="s">
+        <v>279</v>
+      </c>
+      <c r="CU15" s="83" t="s">
+        <v>279</v>
+      </c>
+      <c r="CV15" s="87" t="s">
+        <v>279</v>
+      </c>
       <c r="CW15" s="85">
         <f>IFERROR((VLOOKUP(CQ15,Scoring!$A:$B,2,0))+IF(CS15="y",1,0)+IF(CT15="y",1,0)+IF(CU15="y",1,0)+IF(CV15="y",1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CX15" s="79"/>
-      <c r="CY15" s="88"/>
-      <c r="CZ15" s="89"/>
-      <c r="DA15" s="90"/>
-      <c r="DB15" s="91"/>
-      <c r="DC15" s="92"/>
+        <v>3</v>
+      </c>
+      <c r="CX15" s="79">
+        <v>1.0</v>
+      </c>
+      <c r="CY15" s="80">
+        <v>2.0</v>
+      </c>
+      <c r="CZ15" s="81" t="s">
+        <v>278</v>
+      </c>
+      <c r="DA15" s="82" t="s">
+        <v>279</v>
+      </c>
+      <c r="DB15" s="83" t="s">
+        <v>279</v>
+      </c>
+      <c r="DC15" s="87" t="s">
+        <v>279</v>
+      </c>
       <c r="DD15" s="85">
         <f>IFERROR((VLOOKUP(CX15,Scoring!$A:$B,2,0))+IF(CZ15="y",1,0)+IF(DA15="y",1,0)+IF(DB15="y",1,0)+IF(DC15="y",1,0),0)</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="DE15" s="79"/>
       <c r="DF15" s="88"/>

</xml_diff>